<commit_message>
2023/05/09 Spain 데이터 수정
</commit_message>
<xml_diff>
--- a/src/data/Spain_Category.xlsx
+++ b/src/data/Spain_Category.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjh57\OneDrive\바탕 화면\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjh57\..code\pythonProject\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F11488E-360D-49D0-A6BC-E498BEF679F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7FA676A-F915-43FF-BE5E-EBAF8FCBA1A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28695" yWindow="-105" windowWidth="29010" windowHeight="15810" xr2:uid="{840C3334-2357-4C08-81C4-DABFB40EC72E}"/>
   </bookViews>
@@ -1010,13 +1010,7 @@
     <t>https://a.travel-assets.com/findyours-php/viewfinder/images/res70/348000/348751-Almudena-Cathedral.jpg</t>
   </si>
   <si>
-    <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxQUExYVFBQXFxYYGSQcGhgZGhwcIRoeGxsaHx4eGyEcHyoiGiInIhwiJDMjJystMDAwIiE2OzYvOiovMC0BCwsLDw4PHBERHDEnIig4LzExLy8vLy8vMTEvLy8vLy8vMS8vLy8vLzEvLy8vLy8vOC8vLy8vLy8xLy8vLy8vL//AABEIALcBEwMBIgACEQEDEQH/xAAcAAACAgMBAQAAAAAAAAAAAAAFBgQHAAIDAQj/xABFEAACAQIEAwUFBQYEBgEFAQABAhEDIQAEEjEFQVEGEyJhcTJCgZGhUrHB0fAHFCNicuEzU5LxFRZDgqLSRFRjc7LCNP/EABoBAAMBAQEBAAAAAAAAAAAAAAECAwQABQb/xAAwEQACAgEDAwEGBgIDAAAAAAAAAQIRAxIhMQRBUWETInGBkdEUMkKhwfAFsSOS4f/aAAwDAQACEQMRAD8AWe1PZXuxrXx0gYWpF6ZOwqActoOx+mEnM0GQ6X1MYn2gq36Hni8nrmnpWxlTII8LAgCGHOdJ388K3afsirIalBSaZ8bUd2p7+Kn9pfLcfHGHFmcdpG2eNS3RW2UzOggSAsgsqDUWibEm3M4ZOF8VdAxn2wPApjudQI122EEzz2HIYXc3lmSxMqdmB0r6WG/ljMhWKEETpmSFEAwCBLNyvjXs90Zt06ZcfaTItmcmjZZw1QMXjwt3jDXqW+7DxW6j1iqszwutUUuzU/MAaSJ6jSIM2PQ4YezvH3TQof8AhSqgITFJjp1uCeQUkSCIk84OGbimRTMq2YpgCroPfUl9/wAKvqTqy6l1QLza9sK21ug0nyRewXF6VHLGtWcLTpJ3bKd2cFSFHUkCYjY+WHzgvaNM2lOpTWFYEkdItG9mBN99sU5xnLD/AIfT7syr13qT1Coqj/8Ab6YJfsh4iVepTOwZW+DSr/MRhM2O42vQfHPemH/2n9n9JGaojmO8AtLWCuxHKBB8464l9jeIfvFEAXZeg3ExbrBtsLRuZw71KCVUek4DBgVYdZkEeWKlyoqcPzxpsSRPhYk+JTtpA9kabHz6xivRdQ4S+H+iPWdOskK/tliGlEg7jHNkx3p1AwBFwRIPUHbG2nH0an3PmZRp0Q2THJqeJzJjm1PFFMm4kFkxzKYnNTxzaniimScSGVx5pxK7vGd3b9eeG1nKLZF04zTiR3eM0YOoFEfTjNOJGjHmjHagnDTjNGO+jGaMdqCRyuORprdnMIolvQemJT4W+2OfI05WkWLuRqVSASTEAA+3HT5b4ydX1Psse3L2X3NXRdOs+Tfhbv7A2nSfP5klp7lbtaV0bAKSbNNovz6Yt3gHCAqd4RpkQoAsqAA29AIHwOAfY3s73NPRp1aSGqlIXXUjaeSr1/E4ds7UmkRZSQIAuN+RG/snHzbe1n09b0KXaTPCRSV0S2tx3gQwZgA3Mb8unTHThdVWytcag4p6WUmrqtqv491Xwx0scDc/mmNVtLjSG5OtyNIK+wY23n+xHs1mC/fU9d2pmGnUEb3QYAHU73AO3LxoSc8zXm1+x6k4qOK/FP8AcD0Mq9d+7Qj7RqrXdlpr1bYHYgLqMwdgGIZqZo5emJZUpgMwNQw1V1UOHLcxsflygD2r3eVy7P7i+IlzBrPIB7wxYG0cojYAAVh2q7T1MyzBXanQBMNU1NT2AjWlMkSALHqZjbG7DgWNUuTHlyvI/Q27V9r6mZqlS9KixCie9cU2CydwI3Y8j69QiMaYlFro3N8tmkqBj1KRI9LY1Gc7tSKTVAp5U8xSzCE9TTqAMJ88LucrCobKhJ5il3bT6IYnGhRJ3SC1Tj1aT/Hq/wDfl1LfEzc4zHbJ9ksyyK1hI2LXHrjMC4+n9+QLkWea6uSwsFPTYiA2/rP1tz61U0lWU2A8JEyOZ+/fALhed0OyBGcvBAMXI8JLcgLA6r22BwayeY1MiAq2pZgbGDeJuY1RPMYxyXkun4A/aPszTzBY0lC1edMwFqxEleSPz6H76q4pwxqTGQbGDqEsp5hgxhfWMXfmqQMlTAknzvJPl8fXEHjnCaeYWKnhraYFSJDCw01Y3HnuMPjyOHwBKKmUxlaxBBBJGxjxQCRMQAoJAjfDj2b7RGkpMiI8NzFNtHhUQZcaigIvERyuB49wSpRdgyERcqbxOxUkNKdCowMy+ZZGkfny9TaYMWmMbE1JWiDi4umWp2x4SWoCpTRVpjvdSLFixDd5Y7Fhy21YVOwWXK50UiDpqKQSDBAUat/gR8Rgp2U7SadKFppgwoOw1E6lYe8CGJJMwYnrg7kOCd1mjmaQXuO5cgSZRzHh81iSp6WO2OVt0DZbhfIdtqNfMVaFGIQg979qWhiPIWX443/aFwD95y/e0x/FpXA+0PeUxcxGoDmRHPFQ9jC1PO09RjUGVvOVJ+J1AYvvJ8QSQmqXga1i6al136G8x54z5I6JakVi9caYldguLirS7snxJ1jrcW2POPM4cNGK97TZBuHZ1a1MRRqmQLwD7y+QvO2xN7YsHJ11qIrrdWEjHt9Jn1wrweF12DRPUu/+zVkxoUxJIxqVxu1Uee42RGTHDMVVS7mJ2AuSeUD9c8bvmy7d3l17yp191fPz/Xrg7wjsgoIqZg94/wBk3Uf+xxiy9d+nH9ex6WD/ABvEs2y8d39hNPG6HMt/oN7TjY8cy0Qdcgzq0m0awQBMH2Gv+d7CqdlssTPdx6H88RKvZfLBgAm/lO5jpjNLqs7/AFfsb49J0Mf0v6iI3GaN4L728BveMe5fitJ20qeXvCLwDEHyP39JxYi9lcsP+mPkPywE7Q9k8uw0quggSGHrzA5YP4zqFvafyB+B6CWyi163dAdVxt3eBFUZjKmKoL05s+/16+fzwayObSoJQz5c8ehg62OXbh+DyOr/AMbk6f3uY9mv58Gnd41KYn6McqiY1e08mHQ3wBeKZxcvTasdxZAebefkPywL7B8GetUOZeTUqEimDy5NUI2ESVBHmemIecnP5oU0MUKQlm/lB3md2NhE73GLNyeVWhR1OugBQYUldKqLL4YMARzFzjwer6j2km3x/B9H0fTeyxpLl8/EkZ6kuXpwonQs+pv97T8hgb2MzTu5RySpUuDfclZFzsb/ACEc8c+0PFUq0BUWQHIWJBgqAWBMwI64gdi82f3lTuNLTphjtzj2bwPiMePPI31Cp7bfuevDH/wStb/YiDLPUqd0mrV7za6oCx70h7fj9cMdLMUcpQqM11KnxsC5diGOpwLhSU07TYcoxrxLM0MrTqMQAGZmINy7EsRqi4SQwEDcfOq+0PG3zjmo2rupOmL2lj7QpMAPEbPG+/PFsOFY/iSyZHk27G/aXtG+aqHxFKU2UVQurYAoKrKpHhHTc89geazHdXANMnmorUD6zTapSOOVfiOkHQYG0KxC/JKlSn80XEXhnCXrtqgKvNgqj4DSAG9YxoVJE3sRu7q5l9MF2/m0kjzZgot9cNPDeGJl4MCpUNi3JfJcd8nlkSmy0hEGCR71yCZ57Ya+z/ZA1gj1pSnLWWe8aLWBWIJ5+uG06ueCLnXAu6upM87YzFuUMtRpKKenLpp912Ba9/FJ3Mz8cZhqQu5WWaRVCwhCh9RYzLCdJYkReIIFojpiVmHNN1ZYBU6rAjwxpJYwbRpv1tfbHEOK0Kolio1iTC7q2vkvOFG5AjacbUQGpmSFDgq5YyzFbG8WC8h0g+uNo1hscQDOga8m7gQNjEEC4kRzPM+WvFlqMrqoh9Ji/wD3AqdgfDHqRgWXZ1WCQygMxOykAGBNixKmAORJO+CNCtqFMDZiCBvYibm2onSb+eFUaYW7JFfhlPMU+7cHwjwtENTJm0G5ERKn6HFVdq+ylTLvGm26xdWHWnP1WxxdCUdHiQeGbjnI5jra3w+OI2cWjWplKoDJebxpYcwfdNzfyM4MZODtHbNUz5/ydfQZ3B3HX52PpMbYsfsZ2gQlaVfxIVKgk7SCNLcyLkBosIHPAntf2Qeg2tfErGzCwb+sbK/rY9RhUo1zTO1unL0j3f8AY8hGqMlPdEpQ0jhn+zujN5Z1k0XqppbyDAlG6MBYjmL9cdv2dZ92zlVnZiarByWM+/p5/wArx6DE7sjx4PoovphnUKx5GSBPRgSIPPa82hcB4FUyudnWzotKo9NvdZQjaT6ggSORHpgUnHSwLZ2Wb2k4Ymay9Sg0awJU76WExPQ9R0Jwm/s/40V15asdLITGoxEGGBJ+EfeZkyv2b55hQqNXqHUGYs7zMlg2oj1qEYB9oeC0KuZZmdlMAkIN4gg+yQTtgdPkljmL1GKOSFMsc8Qoc6tP/WvLfnjjmc5l3Uqa1OGge2OdxzwhZHsfQItUqmN97RP8vmRgl/yLlR7Re1vET9mI5cremN0uqbTVGGHRxjJST3RZPDOI5CimmnWpAbk6gSfMnc4lt2myg3zFP/V0xWB7E5X/AO5EwTLXJAEX+Ax2/wCT8mJ1Kx+L3n0PpjNq9DW1e7ZY7drMmN8xT+flOOFTtXkSQTmKfLn52wgnsZlpjuWNubMOc/bHO+PF7IZX/KY841P1n7XW+O1B0D5/z1kP/qU5deZgcsDc923yDMCMwpsIseZI6fH0GFml2UyYE9weoln6yNn6mcdV7MZKCf3aQOcvaPV/PA1naAlW7Y5FgVNZCDyIsZPTn19L4EZbjGQps5pVkAYgxJty++T6YlN2Zya//GAtzL8ttnxunZfKTAywFv5uVh72DHM4SUkgTxa4ODbp8nEdqMr/AJ6fXn8Ol/TAbtR2ppGjoy7ipUq+Hw7qD8JlthGD69m8mTAywJHK/K15a3THNuzNMVKRpZdU/iJcTa8T7RFgeeK5OslKOl9yGPoccJKS7HfsL2eFCn4gNUguSCQz9LXIUW33k4KdteIotHWG8LhQpB3kz4SOq88E82VFJVQCBII2+7yO+Bz8IpVMslPuUZVqEKhYwJWes9bYxTuUXHyjdBqMlJ9hY4cHzGVKUpdhXFtdgGptMmLKIv1+mDbZ2lw2kXZwzlZLE+JyYAImdKKCSAd+u85ncxleH0m004Z2HgWf4kCLgmdMmBe94BBM1jxjilSu5q1mJi4BYhUvJJI3MmQqgDqb4THhUafcfJlc7XY947xipmKhettJPdktsSTOjxsBLG3gPnGF/O5+SAPEwO5gnyu5qP8ADUpxsaj1iKdIWPIDSPgqnbzafQ4YuD9ldPiN2A1ELpEL5aupBA52noMVlKMeRFfYEcJ4AXIetN9lJkn1JJgeWHTgXCjWq00CsEkByosqnckxAsDv0wWynZ06yWSQm+moCWnTZdSiwBux5g2OHzhXD6CropxCwGW28b1I9s+tumHhplvdkptrYAcC7M0qQLKgYSD3lRdRsZHdqOl4F5tc7YJPXqOStNhSBgd68FmOxAg/wzNoaL+dsHKojzgj7x+eI2fowIUCwsL3tsSAfD1kGehw8lYiYA/clWQJaCfEzXJm5P8ACPPHuCFLMPA01mK7g6VaQb76ROMwmgNlacORWDgCF1agoIBv7xb3iNVyZBjGUKzDXTXwhm1lyQQLQRAMFjuFm+q9sCs1xzL5dSaVNqhQ6G1yNySzAX5rbp983gHaCpUdwwQ5dSAoURYhiCAbzI1bdcZzTZPpgLrBnSoDLrLSNwxvz1AX8z5YncDYh0VgQVDGDuFk6AenhfEPQveAapcmQCSwSApBP2iw8U7KYiTOO/DK6isylrkQFYjVuQY6xG/p8eSOZP47xBKNNQ1QKrG5JgqIgXA5mBPnOKp4n2yqV6sNCrEGWEKdLIwS7DSQeXzwc/aZxg6GpK6b6WpsJZgVFxP2WNufP0q8NB9DjRHGmtyM5tPYuTslxYNqpVipR/aDAnXINoiIAHw9TiD217D6JrULruZ3UdG+0vR9xz6kF2YzH+G+tRcAnSPRpU+U7CemLeaoaiU3Bk9eQMRPnG4J2jGanF2iyla3KGoO1JouINx0/LFidkONisrUKjhSUYJUInemRafe5ecDmL9u1fY1a81MuoVwJNMRebnR/wCvyjbFc02ei8GVINxz+Hni0JqXxFnGuBrzL16FNlrMP/8ART1EWDIodpEWZTIO3LqLOFLLUye6d4YIJVCLhRpMkXBlWEH7JwqUMxTz+XFCqxWqrAowNhYggjnOx6bjmMFs1RZc9UqhSVKEWFp1Fx9GI+ODONq0CMuxI7JZgU3c1KzVIBJLadRAFwSpv1BO3xxs2cqvV705ggEj+D/BCEA+ybatuZM4UqGQzKvXgVAvdMF23JQCP74l9n+HVdJ76dWrw6mB8ML0MbzhXrpMeKjb3H/tPnCzClRqtRAuSppg+K4HiUxAINuu+JHZvMDuTrfviCG70lCQsE7oABsbxgfxnhlU1arpT1EbAlVnSosZuMTezfD3XL1A1MISgGlTqCwHG/S43xNOep7bbnNQ0rchVcs1Soan75WW8hVq0gi9AF0wR6yTznBji7BqaqjmiWHtoySQJBgkGJM3F7QCMC6vBGIs5Uj7DLJ33mbYF8RyWd00ArwRR8fjpjxd5VM33ERcWt1wsXNp+6FqFrcYOAUDScBq1StJgJVqIwk7QdOqZ5THljrxen3hC9+9GNxTqIhM3v4SR6Axgd2Z4bXV6b1ahYioPDqpkRK3hRM/HpglxPJk1WNhEbsB7o5H1wbnp/KBqOvk78HqIqsvemvAPiqOrFdJvcKNoMzJwKTILr1nN15mY75dPpo0aY8ox72eyNUCprRFJ7wQtRak6gxm21ybfdjnmuFVe7bQyq2klSHQXgxMnacLKU6S0hio3eom9pT3tJAtR6MpJalUCloJFjBO87HE3s8xUIzsWVrIGJJssyCbmAOe5J2ws57h+dNGhpZdQV1aXpQT3rEQTY2YC2D/AA/L1CcuGC+BNJ0sp8TCGiDtMbYpG9VteBZJaaT8kisrMKtNHZWUj2CmoEPBgsDG/PljhxPilPJZaKlapWdjIDMGLyBYQNvhBvyN/OM5uhkTXrNLVq7WUm/kAs2Wbnr6RireMcVd3NWs2pzy+zPIfj/bFuNiaWrc941xV6rmrXbxchyUHkPhub7/ADE06FTMeI+Cmu7HZfIRufL9Ejw7gbVYq5iVTdU5v5j7I8/lh34J2aNf2qcUQpCKLSRIlRzibttNpwI78DSlpA3B+EooKojEAEsQJdogDbaSQPKcE8xlNCHvP3UuslnNR1JG99KyY2A8sPrZGlQUIF0R4w+41X3kgsd4tYYrztS5LFmGUuZ1QHqGP6l+c/PnjP1K3UUHE+ZMU6+cqlyaTd2pA8VHvVMEjwkvcDUJuNwIBxZvZTtMdQSvUpoxY+BUaSoTdpkjrJIMLcXxXHfWCooUQYePEZBBiB8+fMzgr2fy1SlUDK3dkgKWIBjURPIhd7xJIHLFIVDgElq5LsrCVJEQRIvv0/3wP4jWBbRqIMBtWgMKZ5a5ERz6ix22lcNzK1KSuGBBB8Ui4BIm1ht8Me1FDU1EWkf+N+XpH6jGp7ogtmRKtO5mmT53/BcZjhRL6Rpa3LSbfABzHpy2x5hLDRTWdSsyQulmAJcmCSZmdJgnfpfCdQoLRrKCpq6CCdJi4M6ZgwbYdKOYK2YK68mQCQZm4Mbx54CdqStRQQSNFyGkOeVpHOZ36WtjPB06Zdq9xs4O7VFpvUprSZRNwb0wbhTveBudj8cFaWVGp20ajOm5M3VOfnANsI3YvMUS2mamprEH2dJGkEEGZlunIXw+0VhSA0+Jh02OkR52AwXFPZh1dyvv2iVqLVBTp0waigE1JIIkA6SNntzO1owjMmHXtPlGfM1mj3vuAEfTC7Vy/UY0Y0oxpGedydk/sxmCFK6tjtFwPK4xc3AM1OXLFtcRsIJJAm3mTimODsqKZcgEyIBt6nFu9nmb91BmSdMNp0mFAvHwOJSXvMpHgNUKisSCQGFp5cxfAPtX2RXNIWEJWBs3JrbN+fz6idGkkEnwlnJ8yAet9/u2xMyObNhEiJJ+AJjyuR+WItNMsmUVmMvWytbSwZKimem3MYdeG8ZXNamcoKhUqdXPwqJspj2ZOHDtN2fpZynBgNHgqAXU7w3UeXripcx2PziOywtjEioADHxBxXHkT5ElDwO1FqQaqe9o+OIgnYd2TPg/l8+WJPDnpU0C97RBuLbGDNpUcsIP/KebiSVA/wDyf3xidk8yffp/68XeRMkoyLm4bxei7aTVpLeQWPRCCDa243/HB+k9JUdO+pS9MKIPQESfLxDFBjsbmRvUpdfbx2p9kMz/AJtH/UeXw88K5JsOhl2ulK576jz5+bn/APsfI44V8tSaB39DwppPP2RVki9hFUH4HFRL2HzIH+LS2+03WemPT2MzI3r0RIO7MOk7jlIwNaQ2hvuXNkaFNDPf0jpaTHl3M8/5fqMSM3SV3qMKlMAzuf5aa3+KkYppOxOaBnvKXpqPMR0+OMTsfmjcVKfL3j+I54V5F4D7P1Lny9BVYnvaZnVYfzNUjn1aPhjQ5JSpXvKV0K/6mJ6/DFOjsdm/82n/AKzy2x1pdkszNqqW5d4ed8D2q8B9l6lsV+FhlQd5T8JczyipWSqIv0QjAztFxmnkqaEuj1PcVeZkGT0GK9qdkc3yqKf+8jl9PwwK4n2ZzagklGgc3Jgfr7sB5V8ArD5Z7xLi9StULsS9VzCgXN/dXoPrgxwTs2QQ9Ya6x9mnuFny5nnG3rgj2O7Mabp4qhEvWYQF2sv2R9TzgWxYPDeGBB/D3O9Vhcg/YU8vW3rY46MXLnj/AGCc1HgD8M7OKjd5XbWxjSgvNgPjt/SOp2wzZRG1gsdIGyqQQbGNZiWtBAEAY606IWdyTAYySW8/x6Y7ID8iT8L/AK+uLpGdsgcb1FWVSHkQabQJ9NQj9fOr+PcMGsK1ClRG8qyszecgkACDuDN8WlxpQRDqGHIKSrj5EGPTCtV4RSZtQpNTgndiS1heSxgekHe+M84tzspB1EVMvw8eyq3YdCWP3k/d52wayXA2jxwBGxgmfPTYDbmfhg/QyyoIVQB5c/Xr8ccsvWD6oHsmPyPocNQXI45HgWYrKA1TRREgKJgwdwAZPPxFlPlhny2W7mitMEsElSWkk7ktaIPPpy6HHLgNUd2b+y5G8AWBv88FEWdVh1B9QNumKQgluuScpN7AyKQ9p6E/zLqMcpJaSYjfHuPP3LM8qq/GkrfW0/IY9x1vwdt5PlrJZtiCyHS6+1EQR1jYjkQbfPBVuIitQYPIdB5kA8iOQUnedj64XeEH+Ko+1Kn4gj++JVMFWgH2lIO5tBJmPT4YMopnRYzdjatXvQBVp6ZlgxQk2MadXi3v4THXD5RrSoMQd7XAJv8AQ88IXYrJUqneM6xpHhcTKkgyYLAQBecO+d4jlqCeN4MezBk6YWwgzBFxq64g5RUq7lknVirxHNB/Ekgl5NrEEyPgcdG4QGuII6gzggcquhVINgACRGwsfjv8cSOC8KX94TT/ADT5wp+eApi6RSz+UFNGWLlif/FI+84ttHRMuhIEIAfQAydp5eWK17WUgMzp5a1H1UW+WHbjEvllXcmJnyvbzn8cVkk0rOjybcG4rTzGvRJ7tiT/ADzadoAmQBJtBwSmDAPMi3kCG/AfPCB2JBpZlkgkQyjwkjaReYFwOXLBbi3Gmp5mnSt3Y3v7R2MmbweXX4YiyiG/J1SCbdNtuZ+Un6YXOJcQJrMoUSWJ36NF+nO3pzIGC9POqtVUJ8TEwN7IL35c/jhU4xUAZgDAHiLSJnUTE+o5c53th8cFYJyonvxDaVHht7WxM22jGr5lRqIUbgNflyiPK+BS5oPDkE20sRyaOc7R0xLpO3RiRbY+KTv8PLmBi7iRUgg2bUADQtxI8XIdfPb543ybrUBjwhTuPQGcCqQkFQ1x4la/iEXA6gTePPBLgtcQ94lxM+gsfK2OSXJzb4M49xc0ECpBquLEwdC7SbmDvupFueEus1QvrLVCZ31zsQQI0mRIBg2sOmJvaHMGpUrMCdRlVBN1ggRZ2Ai4s0dN8cgv+Df2RDeK0wdxMm43xmbt2VSoYeyvG2MUqpudtyfU23mSxsBIjDK1XRsJv+pvbc/liveCVWXMJVYmRVGmfFKk2EFlHMESYBjpi5c/xCjURVDB/HOmDeJgX3kwN+eHVNVYrtPgWU4hTNytp+vl4r/3G98daeeQE/wzO5i/4+vyPxOHJ0/CulVZ9/5fJfOTvyEk33kJl1AJWn4j4UBAPhESxB9dz/LgaA6wEucUiQGM7SPr7VrX/RjnWrU2BsdtzFvI+L9fPDSuXpXIUaV9k2uwmZPO/XmDj392SFhVIIl2UWFp8M7fDkcB477hWSjtw7JqtOnIAGlTpAgAwL+Z8z9MTiP19D9+NUZbAWBFrcuX0xA4rxAUtLHYkCLXJN9zB5bX26nF3KMFbIJOTonPABMWE+fp922IoqhwVNm28JGx2ZT/ALHHXNP4Jnl1jzEE2B6T54WOzzt3tSqZEtEFWT1OknQZt4gBcHE55dM4xS5HjC4uXgm8Q7NoKY0u2sm7t4twfdNjfr88RcpwUUjqLamaxMAAAdALCZn5Yac+w0H1H3gYgVBKg+f4TimiK4Qupi1V4q1xTQCObfkPzwL4jmGpUKjxMCSoYjVeLkeRnBRqBDERNz9D+vljnxPIlsvWUqb02if6TGJsdGn7Ls61SnXBUCHUgLPNTuT/AE7wMPqvEzYaR8N8Vd+zLOpT74O4WQkSd7vsOe+Ho8epWCK7zaVQwATzNrDDwlFR3YsouzapQWbZkKOki31xmAfEHyZqMWp1tRMmGWL9PHjMTcpeF/2/8DUfL+h828KMVVYzAk28tsF+Dsv7xTLWUE8p3BABwJ4ZS1sQPT0sTidl6RDgA25H1kffjSyaGvI8KPc5ddI/j19RFxqUK0hovHiHwttiJx+sauZqAkkLUKKOgDEQPXfDpw6l/GyS8kpu3zKgfccIHfg1S07uW+uq2JZIVwUjIl8M4hXagxp1Cahq296AF8pgFhYRcTA6WT2Xy3jUxeHJB5GQPxxVfZcjwSdkEkkmAxMwCSIgfZGwucWZw7ilRKkgKxbpIsSbXB+zcDrjLklUjoZOUxe7c8EdM3TddTitUEeGdDAyQY3G7X5A7xhy4dRWosqDp5GRBHl19cB+IcVavmEDKFVBUaAZgpSaTMA++Prgs/aWlTlAj+AhZgabEAkEGfpikncU7GWzoTshlCvFTZBB1S2qY0biPDE2/viLx3/GVhcnmupp85pwW8jg3xKtSqPmaye7SRVJBBBYv1vvGBuU7mvXpU9akLEgETCJN/KQMFR7BbOjVS/EqZG1PQp+Maot1JG+BHaeuDW7sEQNx1Nrx8BfyEHE3JVQaj1kdatSDUMkG4ICxHQsPlgEiJV4hVLuqaQw3gArU0+8ecFvjhoxYHJBLg2WIVmAlZClfI89jEH0G/lg/wAKy5eCZIFgb+yCYHT6zYYyjk6KUmRaqOahgXUydgInr8sE+E01pqO9emGO1wPCLDcybg/CMFt6QJLULXbmqaT0ChjeY6QPMTe8TuBgvwbO6lDCIdh87Tf1wF/aRUVzS0MCIO2POF50rlw4psdCM8l7EoyqZkT7RHPrtgwdKmCW7si8W4iuXXUSSTZUBiTEn0A5nzGFh+12ZJnUoH2QLfU3xt2wry9ITtTn0LG/1XER+z1cZcZju/4LbNI5EjafLbfyw0YxS3FnN3sN3Z3jv7wyK9nWohIBMMNayR0xd/GWUJq0izzIsTpk8oNyNuePmbslmDTzNNxussAeekaot/Ti7+L8aq1coS9KA9NXlYj+KSoB1TaZEEbA+uBJKK2Cm5Uc+yPFXzVfMM/shV0i8RLeQ6dBAgcsOdANce9EKx6TeepAIjyHlhF/ZjSipXH8q/e+H/MKyrqVSxANhvsduvpb8MTgtrHnzRC4rKoQlgpAAF7kiT+vXEHhlZw6qfFTYHUJuCNMECL2EdAJwZqZZnpwRDTMHyacJHb2o+W/dapYqozIVwpnUpSpMgiGEDYg4Lj3FTG7iVcrXpRYLuRttETB+R0n1tjXjtJmrUgJ0zJI1DYTuvhO0eKPrjWtT76oxCnVT8BnT9lWsY1XDA2MemJFaiQVqPe28SZiOW4vuZOIuDkn8b+SH1JV8KOlRx3JEyQpBtr6+0vMW5XxB4DlAlIADck7MOcbPcbYzhWWWo7oxgyxUgkMArQY6XIvgip0EAwFC+0WG4ixkzJ3xZQuet+KEcqWk557iygFDTba5tEDnFzFt4xtks2lRfBcT7QPlt9cSKQp1JGoEASYblsZg7evl0wMr8Uy9B2RqiCWlQJgzeLCJ8vTDttO29hbVHHMLpZiBJDTHWTMYWRma5pVxUs/hOkwCVZiDEnbwnBl+MA15WSDECDJMA7AEmw3A/stdt6J/eKMf9SjWTc7gKw6bXN8KmpXQUwAuWMSJF9xaIMz62t0w7cCRczTZhSV6iAApVeowaSfELnR7O0GCd4tjhwTsma2Xp1GqQaiKwgA+FqYI35yb/3nDB2P4cMvVqKaqsXAERBkQfrqOOUN9wykjtlezyMisFRZUGDRFiQJ2A548w0UVgfE/eceYrpRO2fGGTqFQSGIE8udsGeGZ7vDTTxHSTFxFypuI6jrgJS/wz54K9k6J79BHn9cUS3QLLUNTTXnlSykn51T+WK2y9NSrXVZQg8okRzw/cazS0xnCR/01pi8b0l/FjYeeK+p5um4ZG0iRCmNOkyIO9+dokzieV00K50qRLyWcFJdIcNAlYg7WEjewi5HpiR/xhkJa6iRchdgfFzkGTyjfAOvmE2lDEQYBBJEEjeORM/K2IlDNvq8Jnl1t5jy87Yg8Wq9hN2PeW46dRfcldNz7rCDB5z8Zj1xNzPiD1QxJgsyzJmfKJP98V9R4pUuC7fON5n43O2GPIcRDKwioWUbAmSGsZUk8+Y64lLHKDXgKcouwxSrVEyVQuV1s1ITAi7IduYGs74FcOrLQru4qeIKwKxzPhnkI9JwW4i6LkmBJ1F1Oq5FirDYb+Hbywm1szqJdEBN5MyOu14J5fnOLxblFDTyX+UZ+HcUWmIKxIAiTsCvszbYdRjhS4Mhq1KgqgtUYtAggSwNjz3N7fTC3rLH+ItTVcyJGwvBnaOg54JZPPCnckg7Re0XtIg+vniemUfyslqkuGFMpxE0ipam0KwaCv2SDKzHQnEnNuMxFRWACUhZhcgGJHLdtsBeLKhHeFiXYxZRexNiLnrfp5nHuTzsMoAIJPswZKknkefUAH6YMJNI6MpLdG/EsqdIf3QQu8XbpG8Rf1GD+XSMg2/+A/ObGumAmb4dVCadFQ8wxQ+5flYagT8QOuGVKDnIEaGn9320mb5gWiOg+WN2hcpdi9iRxPh716qrTEsKagC5k+Jo+scycM1XjzrkKuTegumlQ0sy+0CQxSp7UQToBWJu55YhcIybisWamwXSACbQZpqD5RJa/JTiNnuH5urrOgwUUAGFsqpAItJBncYVRjJ1T2+g9VHVa/kG8K4Y1OshJUgytjeWpMfZsY3vtte+LrRErcOgMyjuqKkjcaatSd/XFb1soyOP4R0wCYuQQpAMmTF4jpHlh44Q8ZQAnSO7WZkf/I5/32wMsGl8hYtWcuz/AAkqKlTUWSAJcxfUBA6b7332wz8CoEOdvYbmea45cJo6EqSwgkMdLSICueUiDH6MRMy/EaVNDUmWbwqqgGPUH7sZ3UI2x5zJWe4eves7H2mgDccrnADtRwCnmqOim4UrVVtZkhYG21yVJtIucdczxVBT1Vu7plj7LOZKi4kKQUtuL8hY4KUcxTpooEKGEiI8NxsRZYkWx588k71EtbYTYSGgrczz3CKpn4g4jVy1RAuoAA2YMRYTsR1EfjgRxvOMEdu8qoBBJRCzDkp0xqAkdDG+IbcTBpogql2Ii4CgusAyLkkHcXiI3wjlOTcgOe4d4FlFSspGqO7dZJsAXpEDrJgm/nfAHj+eqUXfToDEsVB5gNcjkIF/l1x5wzMZkKHYlusMsMQTAFhtvEwBO5N1LtD2kd6iCrKw4IDCDI03DCCvO63gxPPGrHlbjplz6B9pQayPbbu9WsEkrcEREFbCSQR+eBWc7TPUZnEMDNzqXb7IkrInczH3J2Yz4YBVGsKuktKrAHI7GNyb8uePFrTbuwIDXOmL/Ek/SBtg+89iTnJjDW7Rzp1OX0myzpBA5iOc+R+mJWe7QGsaVQqZpO50sL6WWLEKJFxciwtHModbPwdUITNyI0iIt4xqMRMSD547Di71CBoQztEhQQTeB4QT0v54aOOUd0BSkixMtxoHLLoBfu6elgK2mdKwG0k6miAfBgv2U4sBXBYUoggaSxLQV2moQpIIIB6HFWUMzUJjWAgMEh4BYwQBYG/KOZ3x2yOfpmqq1FZEEAsGVSQBeTLQB0BuNoJw0U7sdTbPpFM1ImGE8tSW+TYzFZUMq2le5Y1KcDS9OtCta5A7y15+M4zGi34HKWp8MYDn8t/rgrwUNTfWiSY2MwIJnY7CMOCdm62zVadP+oqD9DOOOU4NQoXfM99vKqrczJAMj7jjRkhGO6ZyjKSoV+JcV1GqGH8RjeSovqXnAC7ESBPKL4XqlByZgKImeQjcyJMSdzif2nzNN67tS26aQI9IA5Dnf5YFtWdhBYwFiNrDYYjT7C6aN6NUU5DKrTYyLj0PL+2NatQnSAoW0WMT6+eNstmGQ+E39AbdJ3j0xIfPpsomNpuOU+1JAtaDO84D54Od+Alwyq4QwtOSIklQNAm0r7RkyRfYYl06pJBUjUDc6ixUdQxsVJ5H5WkCaGbDK0DTAuQ0WMAx9kAgbA73F8S+FMLAKp0gmzEbXIJB0m28YhOPLFaDuZzxAIYHUy2B8oAsFMyDYg7jlhRkq1xEG4a58Q3Cnzk+VtsMFDN0XvUpWIvPikx7sydxyYcvQD8zR1VGcQuom9xctI8v9hhcS02qOpJbkOk0WDRvZhAYgWiTA2tMffjpl82e8giOUk2n0sJ8/S2PEoPqky0GDqO4hSedj6Y9pZTUWDD/ALVO1jsDaT57Ys0gWg3lcxTdSrgKGMAzMnlsT5jccsRnr0qbEoIJbTe8WAEbECb/ABOIdJHjRo3lh5fiRHXHiZFmIWDM2id/K22OxpK7BaTGT/jjKdIqSRuNF5MQoGrc39bYbuF0HNLVUILEEgDwxfnfeOmAvAOzgo/xaniqt1khfTqfPDGaxjQo8TeFfjuY6ASfhh5S1Oono44uMdcn8gPxHOsulQTrckgamsqEBjZgdz/4HCzW7UVkJBU2APt1LyBt4tr7407Q8VVc2xAmmqBFHkki8G4Jk/HAriPGDVD/AMyogBEwiDl0OoT6E4Cm4t72jPNqatrf+7DvwDj7d6UqVJBg+0xgEDqeXPyM8jh5z1B0pF6dyPdkyZPu+ID54pLJ56WWD4tU+zsFQ2nmLbRsfLFudmeMivlgmrxJ89Ow/wBPsn4dcUm1kja5XP3Oxyp6Xx2PMj25alKlZ/qERPK5Mf2ODdXiVXN5YvlnWmYMt4bQSLwCPaHSbEjEDNcIp1UnSA459fI9R+uows8C4xVyBqUqtMBGPsExaSZUxeZPP64yzbrc7ItPIx8Wp10cU8uO5RBJNUoAQJJKyQZtfURsfgU4s7KopKO8qaYeq66F0geIseg1ExPMxfHPM9pqNahVNIl2dSCAskHSYmNr87DzwP4h2wouSUadUqaZBWbAQdwTboIk3xklT3RHatgHmstVNYrSIpaVliYZB4rKHaApM3hRfVe5XHtaiSUZu6apShFqmnUVU03JfToBUSbwBZ7bxKoZpcxpNTTQ8alkNXT7BJUeIaDLqpiZgC8WHue4fXbMU6DZljTLkppKlxC2DAqBMkC7QSb3OKRpipAMdqqwLIXStTew1MQCCXuFaHFgbWNtxIwB45mO8fxCTPtEnopFp1OF2FzYCTiwcx2ZK0nc0KbhbsUJQsFDHVtbVMkeGCPUYq7iIq5cmaZ1SZYgeEA335+VvMbYaEKlsjpKSBdKgqkyxL8/A1iOgAg+mOq5ymRFViCQPdLADVv8gLRiDX41VIALEEdLb8jzwNZp3xp9nfIyg3yMVcgQe9FQruCFkE9Abj+oTy6Y45aoneILLDCJJa0TfUDvHICLWwEU7bH1nBbJ8QUbhVEabLMzufFPy2MRzwXGlsK4NHatmKZABdQZOoIPC0Ne4Wb8iLD64hUs8VZjTJUGZvMibTvB9MeVcszsNCtBmJWBsdiTAHqbY4+yfELjz+Ub/jgxih0lQ25PtPVVFAq11AEABUIAG0HnbGYHf8ZpfZj+koB6gabTvjMdXx+p24YoI9RijVTIAJCoxsxgeJ7dbxgjS4UtMt31gIgtULTIPuppBgx5b3xG4dnA40VA2vvCHGogQoBkxG8gA9GOJFDiT969Nm1BKmsHbwlSVEjkrXA9OmA2/JbnkWuPcOFJnJLClJ0MumWOhSJE3ElhbbbzwtUsuzzpkqpEnncwDE4bs7Sp1NfesRTR20qDAOoIx538UmPPAommtNVWAXK6iASYtvP6k4OrYVqiFWpIFcaj7QBBUSDBOoW9nlaMRqmQZYuJImJ5dPXyxMfLlnYtIUm03O1v15Y1yhWPEZMEAESPaO454FurRLVRARR5x+HW3TE1jENfe+n0O1+f3TiUgDEkKQfhtfaLbc/XHFMqbkCRJsen5zjtV8nawlwqtQYM1UsDf2SABINxMmB6RtOIua4ioYhGLJaCdzt5D7hjgmWUgiCCDEbb9CR+vpjX9zgjTB8iRsB6354TSruxfdb3O+X4pGrzJN/liVT4qu5Hy67ScQ6eWUgGIvz+4T6b4k0cjqaFQEmAPkLERfB0psD0kqhX1sAgJMQB1+MYcOA8LFEBnjWeUez6fnjTgHBhR8XhDcza3kMGlDTM/GMc0uxt6bpknrmt+yNncnrH66Yg5/Omll6teRqvTpR1J8TD9e7jaqxJVFu9Q6QSNurc4j74wP7VZoColBDCUlggcyRP3AfXDL3YOX0H6jJclBdt3/AicZSHH9I/HEGcMGYAqgQ7Bl22v5YFVkqqfe+OM0J2qISW5rkD4/gfuOHzM5hUGWakwVjl01kf5ksAW9VCgg39nrOFTgGT/i0y4BDVFGk8wWWZ8oti1+O8BoCgyomkSVEHkJHvHcQLyOWLYsmmVrfz8AOOpUSuB8QGYpSLMtnX7J/EHBTM8MpZmmadXeLH3l5Sp/XmMVj2U44abCo3Lw1R5D348vunoBi2qUMoKtvdT/fFOoxpbx/K90NCWuNS5XJXef4RVydUMrEAmA4AhhAs0z02Iv1wycI4hk65ivSpLU5+EANbqB1E/jg5mVVwVdQQdx/viv8AtN2cqUPFRlqW/Msm5tzI89xF53x50k72ZKePS7XBYv8AwLKkCVWBAAG0TtHI/USepxC4Q1FKmYTWAgrqUAaynuaTEKBIUamYwQN5xV+V7TZhaZpkEp1O4iJv0t8b4n8B4bUzAdlrhWLSVLEEjaSR4eUQBy88LUlyBNItfOceU0z3VRdZsuo2kxAkAxt0+WPnvthmKgzVWXVmmdSmZJgzfffYz8d8N+ZyGYSpUQajpIgDxSTOnYeRuY2G04g8Q7EVq8sE7th4qj3IgC6hQJ1eXXni+PK/1gl7wi5jMWAUr4Z1MBE65uJ5xNxFoO+IdDLBp1OFgCCeZO1vr5Yf6X7Nay6SdAIksrki0wIgG8Ha+AfE+BvRRe8paHZDUGoGYUMGm0KNWk+WoW3i8csXtE7jgEUuHiStRlUxZiZEmI0hT4rcza56TiNXyPdzqZSwIEAzuDe1+Q5e8PLBShlXqU3daTEhlSwBClyVRWU3lipF9vDtIxHyPDalXwog1TpYEMNJJjTYTM/GY3xVPyzk5Lk4Uc2IB0iVsYYEsDqJIBEW855Y4FY3XxTtcW6C3X7saZtGV2Vhcbx6csSM/TNNyEq94tgtQAqGAVSDpNxExe8+eGilyg1taODEHZY+OMxyjGYIwwUOL6GrOBOp7fID8MQ6XEHl2E6mYbcgB9MR0gbQQZtG/wAMa6iTAEz7oBm+EoVz8Ekkx4jvO55nz+7GXiAsgDy6/nibw7glRoLnQp63PnhkyPCKKj2Q56tfC1QY4sk/gKFKr4dO5BjYW35RcC+NcqQVhtMMTPXcwfyGHipw6lAPdJ8ADP1xxPDaJ2pJH80D+2DsU/Cz9BVZlkxtytyMW8+vrjqta8SAd/MnyiYwyJwuh9gD+mfzx0HCaBNkBjaWI/HC6Exfwk/T6is9UEwzfK4vG/Ixyx6KjgA6SekdIIMTO/54bKvB8vvpA6+In6zjmvBaE2Q/6yPqcdoB+Fn6C3l6RqsAoYnaSBb15enx88N/BuEJSG9+ZicdsjkKdPaAOl2+ZjHSqbyAQOQH6+/FFClsXw4FB6pcnfvhbS23LG1R+Zv8f72xDQ8zjnxFp0ojS1QxERA5/PYYKx2zRkyqEXJk3h1cKKuZb2UUhB6dPM/iuFOhWNQkkS7kktE3MybbXODHbHMClSpZdf6mjnpP/tP+gYX8jUA0z6n7z64n1Lt6V2MEL5fL3ZAeooFyxjoAP1tjsaxkCb9fu5YjZ6lodkIO/SN745s15g+uMekqEMhm5q0yQPDUU/JgfwxafEO0WXqgU0lmaoDDArK6pJmCVtPLFW9ntDZhC5hFMmT+FjuZMG2+Lc4/nkSgHOkjvBbeQTBWBvCyMViqQUxG7T8KOXqmvTgrcuQbMpIv/UDMwT94wx9iONxpy7GFN6R6iCTT+HtL5SOQxDXj2XNIJqjQ0oTs0TKuAYuGj03wqKypVakpZUnVSPvJBm3mjbdQJ5429M45IvDL5ejJZLi1OPzLiaoPXoR+r43pVpBET1ET+QBwv9muNiuulyq1lOl15luTpJ9lheORkYNrUA9oFb+vxgf3xkyYnGTTW5dSUo2hc7QdmA01aAgndJgHrAmAT02PlzT8uTTbw2ZTfyItceXMYtkVVaxO9vEd/QAfdgL2i7NLXXVTOlwLEzcdGEeIeZMgfLEZYyGTH3Rr2c7VKV01jDsR4gANQi0n9RhxFBSLHwzMLF5uTb1NzfFQJwDOBT/BW2zEp/YjEzhfaStl/A6swi0Ex05G+3XE3il23FS8otcUlIhVBJ9AJA6fLlgXneGU2qB6iBmVWUFhrBViCwAO3si8H6xhJrdvWuwolWvu0kC4A9m3I2x4O3zSWKtI5SBNoI2v/vG84PsZ+N/Idhoq9mMtVbvTSam/fGpI8OqqwSXgbnw/GW6zhL4f2LFQcRpUKpBp1XpqWhi6vTplFZjeFI+s74JUP2gTpGixJks0ab2MHYf74BcE7UGnmc4wK/xKiuG1RPg93k1xGKx9pFPuG0Mvaf8AZVlqxapTfuHbQqKqDuxAhiVF2J3sREDHvar9mmRUJVRe6Wn4npgEiqNVOROoMPCrAXsWn1zJ9vWAhwsqZBJEiftH64D9r+Mvm2AV9BQQy05hlJDCTPxm/wB+KRm2g2hOrdkgWJp1dKcgSbddz1xmJdOg8C8+cC/3YzFdxbQtZHgLNd2hegwxZXK06Q8Cg+ZnGYzDybNOGCpSJauGPsT5AwMdhV02IVfgTjMZiRpPWzAiFNvT7sc1pneMZjMMhTvR8yQMauq+eMxmGRxuHMch5AY9CmJx5jMMcdqdSPL0/EbHElaeoSskecYzGYawtHhWBY2544dnFL1HqnYQE8pML+ZxmMxXGYup5jHtuKfGc/31Z3MxMKOirIX8/jiPTciNPLGYzHmybtgOubp94CfeFp6/r16YEBDMSZ/E8seYzCx7hYW4akeI35ib+XwIvfnbBBjN9tjY/L88ZjMc+GFGndqpO17Hn8rY555QRqU+NLr8Btt0/DHuMx0G1JUGSVHahmSVWtTsyiY21LYlfKLEHlbFk8A4qMxRDQJVRJvcESGuLel74zGY9brEqUu5n6f8zj2OeZrEmJIYiRiPS4jVDQYZY32/XyxmMxl7Gpm68RmdSz6+X3b8hgLnqIbqCf1bpj3GYKSGQLr0NBgr8Z/UY4VUA635kz/fGYzFaRzNakixPL78aNV5feMZjMKcczSB2A+WOwokeIeEESQNjF5j4DaDjMZgLc6cUZ3lbkyH1n8QfvOMxmMwNETN7NH/2Q==</t>
-  </si>
-  <si>
     <t>https://youimg1.tripcdn.com/target/100e11000000qc24l39FC.jpg?proc=source%2Ftrip</t>
-  </si>
-  <si>
-    <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAoHCBESEhgSFBUYGBgZGRgZGBkYGBoZGBgYGBgZHBkZGRkcIS4lHB4sHxgYJjgnKy8xNTU1GiQ7QDs2Py40NTEBDAwMEA8QHxISHj0rJCs0NjY0OjQ2NDQ0NDY2NDQ0NjE0NDQ0NDQ0NDQ0NDQ0NjQ0NDQ0NDQ0NDQ0NDQ0NDQ0NP/AABEIALcBEwMBIgACEQEDEQH/xAAbAAACAwEBAQAAAAAAAAAAAAABAgADBQQGB//EAD4QAAIBAwMBBQYEBAQFBQAAAAECEQADIQQSMUEFIlFhcQYTMoGRoUKxwfAUI9HxUnKC4RUzYqLCBxYkQ5L/xAAaAQACAwEBAAAAAAAAAAAAAAAAAQIDBAUG/8QALxEAAgIBAwIFAwIHAQAAAAAAAAECEQMEITESQRMiUXGhBWGBFDMkNEJSkeHwMv/aAAwDAQACEQMRAD8A8PFECjFGK9gkcUEUYoxRimIEVIpoqRTAEUYqRRimIEVIpgKMUwFipFNFGKYhYqRTRRigBYqRTRRimISKMU0VIoAWKkU0UYoASKEVZjrx19KEVG96GJFSKeKEUwEipFPFSKAEihFPFSKQxIoRTxQigBYqRTRQikMWKEU0VIpUAkVKeKlIBYoxRijFAAiiBRiiBTAWKMU0UYpgLFGKaKMUCFijFNFGKYhIoxTRUigBYoxTRUimIEVIpoqRQAsVIp4qRQAkVIp4pWYKCTwMmk2krYJWXaPTG5cCDb4ncNwjgyPnSai1suMmO6xGMD5Vqdm+0+k09vaqOzEd5gEEn/UwJArP7V7e099gyhlbg7lyR/pJrzmH6nKWudxag1Sd913o609Ilp1TXUtznipFNFSK9IcoSKkU0VIpAJFCKeKkUDEihFWRQikBXFCKsihFAFcUIqyKEUAJFSmijSAkVIpoogUhixRimijFMBYoxTAUQKBCxUinijFMQkUYp4oxQAgFGKaKMUCEijFPFHbTArijFPtqRQAkUYpoqRRYhYoRTxWhoOzDdUtMCYgCTyPQRmqs2WGKPVN0izHCU3UVuP2bpbSWTlCsy5CAqNvxyfEY5/SsfU6bTu63rTBgSRhAi4BkgeMkV7W1YhANpBhZwFJ/DkDrCifWszV9mIQqr3ETdtCqu0bnzgRzJNeQwTjHUdTe13+Du5IyeJxS3o8/FCK6NRZ2NtkHjjxIBj71XFexhOM4qUXaZwZRcXT5KoqRVkUIqQiuKEVbFCKAK4oRVkUCKQFcVIp4oRQMSKUinioRQAkVKeKFAgxUAp4ogVGyQsUQKYCiBRYhQKaKYCiBRYCxRijFGKYgRUimijFFiEijFPFGKdgJFGKeKkUWAkUYp9tGKLEV7aO2nipFFgJFavZCEiC4VZbEd7pnJIj5VmxWn2XZJG7eyrkELA8M7o3dfGK5X1d/w/5Ru0P7v4NS1plAYm65ydsKpxHB7mMicRzWXr7f8ttl1uQQGRIHeE/gBP1rSNu2IVnfjg33EyPJ81wazTdww7rJGd7kAE/h3krXlk0dlpmAitvfcQxle8oIB7i9CTFPFRUK3LgLFjuXvNEmUQ52gDrVkV7LQfy8fY4Gp/dfuVxQirdtCK12UFUVCKsihFFgVxQirIpYoGIRQirCKEUAVxSkVaRSxQMrijTRUoAaKIFMBUAqFjABRAogUwFFgKBRimApop2ISKIFOBRiixCxUinAqbaLECKm2mijFFgLFECniptosBIoxTxRiiwK4o7aeKkUrEJFaXZabYcKWaGCrMTDIT5dR9K4Yrc7GYLbz/j/AD2/niuX9Xf8P+UbtB+9+A3tOzPm2O8F35B2fCIB6xPTwNcPat4my6tb7ggghgd0OABs8/0r0KXBLQDBzPgRWbr7JNsgdWX0w6sa8uuTtnlbKgXLgAgBkEeH8tMVcEJwOaCZ1N+3ncCHOD8Atpn86uYEEbSccnxkEQPLNet0WVeBGK3aS/HucLUwfitvZblTpBiQfTNCKs20pWuhZkEIpSKsioRRYFRFAirIoRRYyqKBFV6vVpbHeOYmOvhOK5LXais4XiVnIzLHA+lZZa3FHJ4be/x7FywycepI7iKEVYRSkVqsqEipTxRosCAUQKYCmAquxi7aIFMBTRRYCgUYogUwFFiFAogUwFNFOxCRRinC0YosBAKbbTAVIpWFCxRimijFFhQsVIp4o7aLCjV7L7OtuquwZiTMCAsBsSTzMHiea09P2WgvoAghbe7kkE7iBuEZIyf7Vz6D3i2hJW2FmS4JPU9Y28nxrs0F0EAtcZpUQQoJI55VJA+deYz6vL4rVura+1HZxYIdCdb0jj0+iQ6dO6g33gWmTgMwABkYgDp1+davula9yMIpHdETLDmIwAKS4be0BfeKeg3XAPuRXPp71sKrOkSsgEqSCf8AM33rLPLOb8zvuXwhGK2Q6IfduTM7iPhyQG6Y8PCpqUBtoJ/wSIHU5nHrSPetQQUBnAj3XyJ73NcDunvAGsSpQMD/AC85IIywH+HrncfDNPBYd7W199uAG4p3mIGYIgYjP6Cs9rFu3buMVTYHlpVj3UbgQZ4n61f/ABlncB7twIM95S3kAEeP7Vn9raq37tmVryju8e88eSAxEefgOtXRzSgmovmuCEsak02uDofSW2PeQAm6C0PBC9BBGATurE1KKHO0EDMAxIyRGPMGi2pQTGpjrDovM90SVU/UmvPau7cW4xLoxLbhsacYYwAT8xPWa26bXTxO5NtVwZs+nhJeVUzq7U13uWAgnAMgTzxnjwxVWh7QnatzBbhvwwfgycyRmuDV6xjDEElxO09QoAjjAG5vCrtHfJCkDazFQJAO1VlQI6YH50seuzeL13z25E9LDoo2yKBFWRXPq9QLaknmJE4BjpNeinkUIuUnSOXGDbpGV2lbtlyzieg6GZ58xgD0rk09wbySihlciBkbgCPHx6+VDVdolnLMOojbkbcGW8P6iunsrSo6mfxDd6HcYj7V5iCllzbPdvZnYfTGHGy5NS0+9Q0RPT7UxFGza2qFkmOp5NORXp8XUoJS5rf3ORPpcm48FUVKeKlTsiNFECiBRAqtSJUACmAoxTAU+oVCgUwFECmAo6hUCKMUQKIFFioWKMU4FECiwoWKMUwFMBSsKEijFOBUiiwoWKkU8VIosKO21YX3avkkqwAXbu3bsDf8SmBAzGR4Z1Lqfy12pvIKhVJC4MSdzA/CATHXiuDT6hgiqiFiOSQygzPwkrBj1rSL3ioKhVGMOsmcgkFbnHyryedvxZe7O/hS6F7INtH3yFEANuYHaQQdqqqAbSCAxJPUjpwNe14rFsKXlQouHuZncWCcwoMDxNS3avn8Sfl1mPhMD+tXXdLccchcREhgRPQtbqnct2Oe+t93RRt7uDvJYbAFJ2bTIeXA3MOF86XWlgIJg7YMGCQoMwRkTEfOrUsOCf5hkET/AMswY8NmKS5bdwsMpgfFwZBg4gj7UmMzydSlkIyIXbJRHYWw8dwGc7CYmOsYIJNDtW2RpypVQduYyu4gAgdSuOvjVu1wfiJ8MoPt7qubXm61psBpj8YkZyRCAU/cVGFpbDk2kg95Qz46MBiRBPoMgsORWDrGHvLlsSCzkd3E4ED8wPM+demXVXFYMUJIxgLwCDE7yYwOnSsBdCL9/UAgiChBIhg2DEdPhFXYscskqSK8klBWzFFxg4ZhG1QIOcEjvepJP1r0fY+jIHvGMkiAIgDMzHjP6VzdlpuF1nQSgKLjggEkD6j61voMD0FdPQaapLJL04MGpy+VxXqKRWT21c2lVZiFjc0QZE+B8P61sEVmdsaE3VBHKho+cf3+VbddjlkxVF/7KNNKMZeYwtQyBtyjuBIEgSxV2ndjJzW52ZbAQkRljgAADEYjHMn51hIj3LhtjqGHnOZk/wCn9K3uyLRS0FPRmH0MVzfp2OXiKT4VmzVSSg4+x1xSkVZFKRXf6jl0JFSmipRYUSKYUBTCqeosoIogVBTCnYUQCiBQFMKLFQQKMVBRp2KggUwFAUTSsOkIFQCgKIosOkIFNFBBJj9CfsM1o2OzgT3t7D/oRv8Azj8qqnqIQ5ZKOGUuEcEV0JorjCQhjxOB962bNlE+C08+LW5P196IrpQtztaf9f5F2FZZ66P9PyaY6X+74M2xpjtVSSCpyJESZkY5ENPy8q05wVjpgzHIwJ+dc1wHcJmd3XnpXS1vu7vqa4U5dU3L1bOnCNRS+xm+zHZ9yxYFt/wtc2y4Y7DcYpmT+EithWhZYjxHXHhVFjAJPgKe78CgfP06TUL3HR5n2b7Ku2NTq7rlSt5y6bSS3xuw3SAAYfxNb952A4ER9+n1prduTtGKZ3BhfGP0/oKJNt2wSrg8zrNA13Wae6SoW2LpPeg7mUAbR1E8/KtPUpFvdj8PoROeRTva75POTHlPP6UNUg91BIn+h8/lQ3wSPPNbRbr3AQSfdIomDtBulgBzyy/asuz2ili5fDqSS6nds3Y2JA5x16da1f8A7JPE/LJrr9n7mxtUe7tFy3JYkZ90nSDPFXYpNSu62KskU40edXti2Ve2GILliF2Ru3KAJIGPrWza9p9CUCu5JAySjzP/AOaL9qJ7u6oRTudzPXLCPyFbfZGlOq/mPZtLb4nYGZ4jA8u7yaujk32ZW8e255Vu1NMzHbcWCTHIwTjkVa99F5dB6sJ+nNbnbnsu7lRYt2+D3oVCCIjdA7wx04zWPZ9h9UJ3van/ADNIA6Rs/WtkdfkTp1RnlpovgxtFatpfu3N6d4jbLKJlVLEEnOZH1q/S6hQjsSCPeXeCDgXGjjyitmz7Iu7MnvrYKbQTkg7gTj0muTs32Wuvp2db6KouaiVIMtsuup+R2feiOqSXl+/H3CWFvn7fBiaTtRjcIciOgjz/AKDjzFa4YESKwrGjd3deGVVIPqSOR1x0rX0KOLY3zu6gmeMc1q0mTJVST77sozQit4l1SjFSttlFFamnFZtv2gQYOnT4YncZBmS/OT5Y8MVy6ntZmMICqzgmC0efT6CuZ+vxpXuafAZu7gOSKsgjBGfDzryDuCJdjPWc+gk/n51amve3w+YMBgGXI8GkHBqlfU278pP9P9z1U1dZtM7bVGfp+dYul19tkQe+Cll75ZHfa8fCIZeSQJr0HavtXqNOwtrdtsogEpZyq5knc5lgBxjMVa/qCrj5D9MvUu0dnTi6tm+zh3MLt7qKACSXZx5YjB8a9CvY2iSD7yf8zpE5xivD+0Hbtq4iMO/d2De+MxuIQpEA97PoKx7N9iPjRTBgNamSpBgFRnEjwrLLVyk27otjhjHarPoXaXY9oKXsXEMSShdTMf4SOvlXny2KyNF2nb3EXrZZWYyVhGC7QFWIg8c+Bp37XtgkBWKyQDI46Vfg10Umpy+CrJhTdxRrBqO6sT/jBHKj0k49cVavbCQJUz4D/er1r8D7/BV4MvQZr/ahuG1p7jlRBm3bUAbv8TEEA+prWs+zvbbiW1JTydxP/YhrzvbGq/iUS0ZFu2zO6g/8xjG3dHUKIHrTdne2d+1bFpHcKFIXd3iBOILyYHTwHyjlZc6cm4q1ZtgvKrPTL7Gdpt8evYf5XuEeXRawO1PZ7tO0x23tTdQMV3o905HQqGJFc2p9rLtxhuvOSslYcLEiPwxmK9N2b7atatkOgcksxdjEyZggDwqpZm+VRPY0OyLNy3p7SXiwdV7+8kvMlu9OZg9a0tPfB7uZjrXB/wAZs3HQlgGvlwgEkHYJOYxjx8a2dLG3OcDpVTTbsuTVFLu20/fpTadzt4PT9/vxqy6oIxA+3jVD3Bb/AJjNtRUJYn4VVRuLE+gqPS+olaodWeX9e76bF/8ALdXObqpAWZ2yfCcY/fjWR2P7baTVXxYQXFYyEZwoVyMxhiVJgxP54rSuyT3RBgRtiY61KSaYotMDtuIgEDr9Dz4ZqjU3gbbKdwKjwxmP612WrkgkiJzHMGuHtKGWCYg+HIn19aVbIZjM2DjwgfpXR7J2bOo1Gpt3E3RsuASREIEIlSPpXNqe0rK3005ne6kiBK/iiT4nafpVXZGpe3d1CrZ37hbUtKgJIKid3iY+lXR2e/oQlujcXTaT+G1AFtC6vqtp2yyqjuEIJ8FC9a1bHaIBtW7SG2t229xEKImwpHdZNp2klvlXl2s37dp2/h1IZHl9wIRQ7iRIBkEHicAeg7wuuMRpLawIG665IB6DGBjgVOLtEGje1CWrgdHcqRcO2LhRowOhB25NeX7SS5bulhpbjW0JJLM7h0GSSxcjjw/2rut2u0cpstWwwIYyXgMCCdsAtjxIrXsqV0/urlxXco+doTcM5CScAEDmoSlFOnzVklF1ZlxvF0oioQLARbkwgO9GnYZB7sCGPQ+g9k9NbGkm6yb/AHl8jLCAbjwDJzn7R61V2fp7/vrirfIIiTsUyPeXRxIiIJ+dP2TptQbCFb4UNuYKbSN8Tsx5YE8z86IZYyXlFKDXJy6TQ2jqb5ulEG22UCsFQljcLKs5gAr4VwsiqJKvxnInr0itLtHR3DcDXHDHbhggSACe7G4zyTPl5VldtAqr3ACQqs0bomFJI4PNanqMjqnXsypYYrlFX8XY/wATDy7uPtUri0Nt7lpLgUAMAQN3E/KpVfjZvV/5J9GP0PNnOOmfp5/vrQ2mI+8evShHdgiDHI/Ska4AuennJP2rPRABbk8DoR+tXb0C74OPAEcHJ70jBqvTkOePKYxXPqEdAFJldxA9ZkyPCpJW6BGtZTcEZngfFyQTiRx8J4xzmtnW9qWyJVyz92XYYVNwO1FHJkbt32rDtWrfupCQPHq79dvlP2qvTWirlioO1ZAJG3wg0NVtZKnykaN/VOCXVVG7naIzGSRwD16DyrPtatywnMST5DBqxw9w5/0iQJnM5wABROhIB4kZieRiOuMT9Kj1RWzH0tqy3f7zMieveBMfuKre8FExGfED5zV3vyqqgg/CdmJAjvSfI+NZ+qBODnxmdw/c1Gk2QJduGSxaevr6z510LcChV5OOuCev5VzKB0k+AkZ8vOr00gZgxaD08Dt5H0ptJ8gM1yQVgZ4zn9KqTs53DE9ADuGYyP8AaupCgARIOcsMsYJJjzEiu5LZJLMdqCdoXAgjG4E+pmkn08Dsxk0rnulABiO5tE+M8muy2RKgERBRl8RwRHM1YdS1xnghWUBV3cNEZY+g+9X252blYb1UmcbZ2kiBMzuzHgCKG2C3PV9k20t6fSh070wsn4GBJ+uIr1OjbkfOPD1rD7Css+ns+8ALDcSYGG3Nn6Vfqe20tSvxMcLAngruLEHjPHl0ob4LuEbCzHe/f0rN7dtbtLfQNANm4sR4owB8f7V5v/3LfO8zElSoiCJxAVuVMk/0xW37P6oXbZVmBI3qZ/EZmVzLCGGfWo9VyHGSex5T2Z7HtWtWj8hWaNysCCWEGY5Efc17B3/mShjuj6/v8qu0WiCncYkO56TG8x04ikuKA3BgqcgemSalJ+o/YdOBHz9IP6xXNrQoB3LIIG3IGRP24ruVZFZ/ajKUKkGQD0PIzzSfYEeU2qO0t+DNnaoJyCQx3fQEfOtXsO+lu9qrj/AqaUuTEAB3knwEA1XqtPLK691gBkATHUHrwTSdmaYXH1dtiQHt6dWI5g3HB29OtWpkaOrs7tgXuz77x8Ki2CYjvK2fMb3Y/OupvbDTkrcJMA7gYaCFTYB8Pi7H1FcXYmksr2Td2DJsq7s2d1w2VeR/lLgDw21vjs7Se6S6dOgchQiFFkFyIUiMcyfCDTi1v7kX2G7D7Q/iVuXh8LMQnPwqirwf+oNWPrtZpmuLeYqLllnQAuoaGW6hxMkd4ek16TSPb3PbtKAtslDAAG4puaIx+IfOaydTorYYWzpkcXPeF7p2BkLb2GCJbgCQaoteM/Ym/wDz+SvsTUrcuXLg4ZFfno13UEZ61f2Klv3WnuFFLe6G1zEoGWSPnxXBoimne6kwFs7F8ytzVQMdYrV7MustuxbUKVFpNxLwwhAAAsZ46kUtP/VX/bDyVtZkdu9trbvBAqtC8kkcqYGOk1l6rtzT3Ea3cUoj7kYh5ZVeBIEGSFLdOgrS9pVnUL5qP1rwV0Xb1sMTO1d8bee8ykCPSr4TdbdhTikk+7NO1q9CqhVuXgowJuIMfK2aleXJI6EeqmpV3iv0+DPR1NpmRe9iTkj5D85z51RqrI2zIEiRB6VqgsRDdc/6fD6UiWVPCgDyxxMetZFkrdjo57dmFCJMcn5jkn99M0E0pJ3RM9CYgHkzHOPyrrZRO3bHy5py6nA6eGBnxil4kuwdgsnAAxwMjur4+pIH18qrFsAjcABPOI/fH1p2KAQfSPMx9+KRGAHBB8T19D15oWSQWOwIXeBJZgB1gEwPl1ptOcb2fYgjcOs7QBg/lXO15maMjjnr6CPWrbNwBwSApJAMzxwdoHqc+FDbHYhss4L22CgEwWkSqwvI8zSPbI3u0Egy8xmfP+lPdWztgTIIIIJiJkgjg5mq7t0cxMkkqfOOPAYFTi7CirftZhtDYWIMmSc58RNaKWWjcFGWwSQIkflyJrhuG1jZb2mTMs7SZw0FjGBXWwbYELfEFG7dyJnw8zSkCR1aXRKuSdzTuOMQegzng0l+2TO07dzDaclduCcnjk/uKp/iCq7c9PEwYMjPQyPSBTLdnuHIJECTI4AgjEkmfpmBVdvkQdTbW3bdWXex2ZE8uDgDpG0fUeNcttzbQrtIJBJMw0gkDcDkCZrpTUgvO1mAPiTx0mBA/foN63AN67mjAb4txPlmJPXxqSe249j3nYnaVpNNaLsAShfbkmBuJiOeDXk9VcTc7oXCsW7olRHDERO7gjj6TUva1P4e2gLhreJEKhQkg4k5Aj13EZzWYrlwcyAB3YO8E+AmIG5eB6xSe/A5SsuuaokTAPQzgpA7vHOTPp4c119l32W4FRzClSCzhZaGMFwRxHngnOYrP1GphVaCQTtgKJMrmMEYA/OuXR2yFL91gSwwJg4z3Tic+MU62I2fSr3tFZWQklju3SMDBZfvjMViP7R3NmwmSveDqTkADBA7rSf1rzhc7WJJhOY8cncQ3y+lc76rCyygcjrkDkjgcxHqfGlTluS6me+7E7dVki80GAQSIlTOTxkERAHSuzVPbuLvVwQfAgyf68V86t6xiw2kAEQ4boONwgYJBI8pNdT6y2pZklcyogEKT1k/Pp+KiTlxRKMqPWuFGZ8ug6xXnNT2x7i5c2AMLltFmT3djs4IA59KxzrHLgsQIBCxMQYO3PSc+XSqrl52JY7SSeCogrwAfqRVib9A6jX0N7U29I1oK2xiio3d2vmH24lpCqPIHpV79oa4sHi58ZZF2BcQUA3bArgzMzWDc1Lj4BsXGASeLeycnrzHE5Fej7H7buJsKIQEARFLAKonMlhknknkk9Jp9XTZC2bnZdrV6fR3ffWnV3Yy7EGTc7pfakkQCPDjpXPqfapELW2V3YhQjK0BH27WBByZM9PxVR237S6k23QOQrclAFZVPIEEwPMEn0rkfUdlLaJSyxuIFAksvfJwZ3Hqd3zNJSi31L2JqSqmb2uMNqnCzFi4wOMAO5DD5PyK79S+qQAJprj9xVDBkAUgEHDETiK8lY7RZbb2tgVTZezEudiuQ0S2ccAHpXTd/wDUDUW9qG2NxO7dJgqHkqJHw4K+nnRiUVtFhKXUzg9rO3P/AJBW0oXYdrEEGSAdwiIkHHXiuTsq7KnaPhlccc7pgnrJPzrGvWLtxmuLbYb33KI7sMWPd3cjIyPCuvsR7i3fdkE7hxI5Ejj9/rUlH0GpO1fBj6xQbjbo3bjOOs1K0bKMo2tbYMCwI2HB3HHxVKsqfoV39y5rsnZ55nw5+dD3kkgL0Hh1/tUqVkaQh0AGfHn1IwKm7GPM8ccfXijUqIilkOBI5zA5HMfvxpiZEL0jwgA/epUqTAQ3yF+Z+k1S9zOc+Y5+9SpVsUPsVqQf9/36UWMesfapUqXcZ2WCq294PeI8OuT/AEpmAJyvJOOeOnMdPy5qVKqlyRZSLhJBOJ7sYgBnxAA8OaOpvwCBO494DnMxM46njyoVKkktgEsNtXY3IksSS0DBP5dOv3utWgCTABMMQMYwQMecGpUpS7gWXrzYZmU7ZnByDniMn18aa3eJAaZ8QJEcsVB6jzxz5RUqUmlQFJIYgklSxMlRmYIByeYx9KVEffu3syNuyYXvLHxAHPESBmpUp9gOhyWIbBBAGcgTMNnJI4rmu6VIYCfwtI429BBz4n+wqVKIDEtnaNxIMsDO3KmJxPPP9qN8kwTmZE+JBMzNGpU3yBUT0NAtHU+v50KlMl6j78Yqy3eIkD7wfnUqUpJCLxqhALmYIjE58B1FIubnMDuRzgrgfejUquSSWwjstXGFuCWYkypmGJzJJmP7U962GRS9sEERMhWwc5XPXxqVKgtmSRxaxzsW0rFCOssSFP4QZwMmspNKQdwOZ54jx/WhUrVCchchuXtQST7xvmZNSpUq7xJEaP/Z</t>
   </si>
   <si>
     <t>https://cdn.hisour.com/cdn-cgi/imagedelivery/PJiouRWxFR9baI5eaOAFCA/www.hisour.com/2019/11/Palace-of-the-Marquis-of-Santa-Cruz-Ciudad-Real-Spain.jpg/w=960</t>
@@ -1467,6 +1461,13 @@
   <si>
     <t>https://upload.wikimedia.org/wikipedia/commons/2/24/Santa_Maria_della_Salute_in_Venice_001.jpg</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://youimg1.tripcdn.com/target/1003050000000pw2bA5D8.jpg?proc=source%2Ftrip</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://youimg1.tripcdn.com/target/0105g120008j9og1mA7DA.jpg?proc=source%2Ftrip</t>
   </si>
 </sst>
 </file>
@@ -1524,7 +1525,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1533,6 +1534,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1851,8 +1855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC2BC2C5-574B-4153-8F69-7B7ECA9C0D99}">
   <dimension ref="A1:E337"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A315" workbookViewId="0">
-      <selection activeCell="D329" sqref="D329"/>
+    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="E111" sqref="E111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -2641,7 +2645,7 @@
         <v>4</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>277</v>
@@ -2658,7 +2662,7 @@
         <v>4</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>278</v>
@@ -2675,7 +2679,7 @@
         <v>3.5</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>279</v>
@@ -3321,7 +3325,7 @@
         <v>4</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>315</v>
@@ -3338,7 +3342,7 @@
         <v>4</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="E108" s="1" t="s">
         <v>316</v>
@@ -3355,7 +3359,7 @@
         <v>4.5</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>317</v>
@@ -3372,7 +3376,7 @@
         <v>3.5</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>307</v>
@@ -3389,7 +3393,7 @@
         <v>5</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>308</v>
@@ -3408,8 +3412,8 @@
       <c r="D112" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E112" s="1" t="s">
-        <v>318</v>
+      <c r="E112" s="3" t="s">
+        <v>468</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.4">
@@ -3426,7 +3430,7 @@
         <v>55</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.4">
@@ -3443,7 +3447,7 @@
         <v>55</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>320</v>
+        <v>469</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.4">
@@ -3460,7 +3464,7 @@
         <v>55</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.4">
@@ -3477,7 +3481,7 @@
         <v>55</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.4">
@@ -3494,7 +3498,7 @@
         <v>55</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.4">
@@ -3511,7 +3515,7 @@
         <v>55</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.4">
@@ -3528,7 +3532,7 @@
         <v>55</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.4">
@@ -3545,7 +3549,7 @@
         <v>55</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.4">
@@ -3562,7 +3566,7 @@
         <v>64</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.4">
@@ -3579,7 +3583,7 @@
         <v>64</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.4">
@@ -3596,7 +3600,7 @@
         <v>24</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.4">
@@ -3613,7 +3617,7 @@
         <v>24</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.4">
@@ -3630,7 +3634,7 @@
         <v>24</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.4">
@@ -3647,7 +3651,7 @@
         <v>30</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.4">
@@ -3664,7 +3668,7 @@
         <v>30</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.4">
@@ -3681,7 +3685,7 @@
         <v>38</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.4">
@@ -3698,7 +3702,7 @@
         <v>38</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.4">
@@ -3715,7 +3719,7 @@
         <v>38</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.4">
@@ -3732,7 +3736,7 @@
         <v>38</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.4">
@@ -3749,7 +3753,7 @@
         <v>41</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.4">
@@ -3766,7 +3770,7 @@
         <v>41</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.4">
@@ -3783,7 +3787,7 @@
         <v>41</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.4">
@@ -3800,7 +3804,7 @@
         <v>45</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.4">
@@ -3817,7 +3821,7 @@
         <v>45</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.4">
@@ -3834,7 +3838,7 @@
         <v>45</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.4">
@@ -3851,7 +3855,7 @@
         <v>45</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.4">
@@ -3882,10 +3886,10 @@
         <v>4.5</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.4">
@@ -3899,10 +3903,10 @@
         <v>4</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.4">
@@ -3916,10 +3920,10 @@
         <v>4.5</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.4">
@@ -3933,10 +3937,10 @@
         <v>4</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.4">
@@ -3950,7 +3954,7 @@
         <v>3</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="E150" s="1" t="s">
         <v>286</v>
@@ -3967,10 +3971,10 @@
         <v>4</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.4">
@@ -3984,10 +3988,10 @@
         <v>3.5</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.4">
@@ -4004,7 +4008,7 @@
         <v>55</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.4">
@@ -4021,7 +4025,7 @@
         <v>55</v>
       </c>
       <c r="E156" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.4">
@@ -4038,7 +4042,7 @@
         <v>55</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.4">
@@ -4055,7 +4059,7 @@
         <v>55</v>
       </c>
       <c r="E160" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.4">
@@ -4072,7 +4076,7 @@
         <v>64</v>
       </c>
       <c r="E161" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.4">
@@ -4089,7 +4093,7 @@
         <v>64</v>
       </c>
       <c r="E162" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.4">
@@ -4106,7 +4110,7 @@
         <v>24</v>
       </c>
       <c r="E165" s="1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.4">
@@ -4123,7 +4127,7 @@
         <v>24</v>
       </c>
       <c r="E166" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.4">
@@ -4140,7 +4144,7 @@
         <v>24</v>
       </c>
       <c r="E167" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.4">
@@ -4157,7 +4161,7 @@
         <v>24</v>
       </c>
       <c r="E168" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.4">
@@ -4174,7 +4178,7 @@
         <v>24</v>
       </c>
       <c r="E169" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.4">
@@ -4191,7 +4195,7 @@
         <v>24</v>
       </c>
       <c r="E170" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.4">
@@ -4208,7 +4212,7 @@
         <v>30</v>
       </c>
       <c r="E172" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.4">
@@ -4225,7 +4229,7 @@
         <v>30</v>
       </c>
       <c r="E173" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.4">
@@ -4242,7 +4246,7 @@
         <v>30</v>
       </c>
       <c r="E174" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.4">
@@ -4259,7 +4263,7 @@
         <v>30</v>
       </c>
       <c r="E175" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.4">
@@ -4276,7 +4280,7 @@
         <v>38</v>
       </c>
       <c r="E176" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.4">
@@ -4293,7 +4297,7 @@
         <v>38</v>
       </c>
       <c r="E178" s="1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.4">
@@ -4310,7 +4314,7 @@
         <v>38</v>
       </c>
       <c r="E179" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.4">
@@ -4327,7 +4331,7 @@
         <v>41</v>
       </c>
       <c r="E181" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.4">
@@ -4344,7 +4348,7 @@
         <v>41</v>
       </c>
       <c r="E183" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.4">
@@ -4361,7 +4365,7 @@
         <v>41</v>
       </c>
       <c r="E185" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.4">
@@ -4378,7 +4382,7 @@
         <v>55</v>
       </c>
       <c r="E192" s="1" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.4">
@@ -4395,7 +4399,7 @@
         <v>55</v>
       </c>
       <c r="E194" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.4">
@@ -4403,7 +4407,7 @@
         <v>34</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C195" s="1">
         <v>4</v>
@@ -4412,7 +4416,7 @@
         <v>55</v>
       </c>
       <c r="E195" s="1" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.4">
@@ -4429,7 +4433,7 @@
         <v>55</v>
       </c>
       <c r="E198" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.4">
@@ -4446,7 +4450,7 @@
         <v>55</v>
       </c>
       <c r="E200" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.4">
@@ -4463,7 +4467,7 @@
         <v>24</v>
       </c>
       <c r="E202" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.4">
@@ -4480,7 +4484,7 @@
         <v>24</v>
       </c>
       <c r="E203" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.4">
@@ -4497,7 +4501,7 @@
         <v>24</v>
       </c>
       <c r="E204" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.4">
@@ -4514,7 +4518,7 @@
         <v>24</v>
       </c>
       <c r="E205" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.4">
@@ -4531,7 +4535,7 @@
         <v>24</v>
       </c>
       <c r="E206" s="1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.4">
@@ -4548,7 +4552,7 @@
         <v>24</v>
       </c>
       <c r="E208" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.4">
@@ -4556,7 +4560,7 @@
         <v>36</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C209" s="1">
         <v>3</v>
@@ -4565,7 +4569,7 @@
         <v>24</v>
       </c>
       <c r="E209" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.4">
@@ -4582,7 +4586,7 @@
         <v>24</v>
       </c>
       <c r="E210" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.4">
@@ -4599,7 +4603,7 @@
         <v>24</v>
       </c>
       <c r="E211" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.4">
@@ -4616,7 +4620,7 @@
         <v>30</v>
       </c>
       <c r="E212" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.4">
@@ -4633,7 +4637,7 @@
         <v>30</v>
       </c>
       <c r="E213" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.4">
@@ -4650,7 +4654,7 @@
         <v>38</v>
       </c>
       <c r="E215" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.4">
@@ -4667,7 +4671,7 @@
         <v>38</v>
       </c>
       <c r="E217" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.4">
@@ -4684,7 +4688,7 @@
         <v>38</v>
       </c>
       <c r="E218" s="1" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.4">
@@ -4701,7 +4705,7 @@
         <v>41</v>
       </c>
       <c r="E219" s="1" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.4">
@@ -4718,7 +4722,7 @@
         <v>41</v>
       </c>
       <c r="E220" s="1" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.4">
@@ -4735,7 +4739,7 @@
         <v>41</v>
       </c>
       <c r="E223" s="1" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.4">
@@ -4752,7 +4756,7 @@
         <v>41</v>
       </c>
       <c r="E225" s="1" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.4">
@@ -4769,7 +4773,7 @@
         <v>45</v>
       </c>
       <c r="E226" s="1" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.4">
@@ -4786,7 +4790,7 @@
         <v>45</v>
       </c>
       <c r="E227" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.4">
@@ -4803,7 +4807,7 @@
         <v>45</v>
       </c>
       <c r="E228" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.4">
@@ -4820,7 +4824,7 @@
         <v>45</v>
       </c>
       <c r="E229" s="1" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.4">
@@ -4837,7 +4841,7 @@
         <v>45</v>
       </c>
       <c r="E230" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.4">
@@ -4854,7 +4858,7 @@
         <v>49</v>
       </c>
       <c r="E231" s="1" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.4">
@@ -4871,7 +4875,7 @@
         <v>49</v>
       </c>
       <c r="E233" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.4">
@@ -4885,10 +4889,10 @@
         <v>4</v>
       </c>
       <c r="D234" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="E234" s="1" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.4">
@@ -4902,10 +4906,10 @@
         <v>3</v>
       </c>
       <c r="D235" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="E235" s="1" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.4">
@@ -4919,10 +4923,10 @@
         <v>3</v>
       </c>
       <c r="D236" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="E236" s="1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.4">
@@ -4936,10 +4940,10 @@
         <v>4</v>
       </c>
       <c r="D238" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="E238" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.4">
@@ -4956,7 +4960,7 @@
         <v>55</v>
       </c>
       <c r="E239" s="1" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.4">
@@ -4973,7 +4977,7 @@
         <v>55</v>
       </c>
       <c r="E240" s="1" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.4">
@@ -4990,7 +4994,7 @@
         <v>55</v>
       </c>
       <c r="E241" s="1" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.4">
@@ -5007,7 +5011,7 @@
         <v>55</v>
       </c>
       <c r="E242" s="1" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.4">
@@ -5024,7 +5028,7 @@
         <v>64</v>
       </c>
       <c r="E244" s="1" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.4">
@@ -5041,7 +5045,7 @@
         <v>64</v>
       </c>
       <c r="E245" s="1" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.4">
@@ -5058,7 +5062,7 @@
         <v>64</v>
       </c>
       <c r="E246" s="1" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.4">
@@ -5075,7 +5079,7 @@
         <v>24</v>
       </c>
       <c r="E250" s="1" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.4">
@@ -5092,7 +5096,7 @@
         <v>24</v>
       </c>
       <c r="E251" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.4">
@@ -5109,7 +5113,7 @@
         <v>24</v>
       </c>
       <c r="E252" s="1" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.4">
@@ -5126,7 +5130,7 @@
         <v>30</v>
       </c>
       <c r="E253" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.4">
@@ -5143,7 +5147,7 @@
         <v>30</v>
       </c>
       <c r="E254" s="1" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.4">
@@ -5160,7 +5164,7 @@
         <v>30</v>
       </c>
       <c r="E255" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.4">
@@ -5177,7 +5181,7 @@
         <v>30</v>
       </c>
       <c r="E257" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.4">
@@ -5194,7 +5198,7 @@
         <v>38</v>
       </c>
       <c r="E258" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.4">
@@ -5211,7 +5215,7 @@
         <v>38</v>
       </c>
       <c r="E259" s="1" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.4">
@@ -5228,7 +5232,7 @@
         <v>38</v>
       </c>
       <c r="E260" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.4">
@@ -5245,7 +5249,7 @@
         <v>38</v>
       </c>
       <c r="E261" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.4">
@@ -5262,7 +5266,7 @@
         <v>38</v>
       </c>
       <c r="E262" s="1" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.4">
@@ -5279,7 +5283,7 @@
         <v>41</v>
       </c>
       <c r="E263" s="1" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.4">
@@ -5296,7 +5300,7 @@
         <v>41</v>
       </c>
       <c r="E264" s="1" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.4">
@@ -5313,7 +5317,7 @@
         <v>41</v>
       </c>
       <c r="E267" s="1" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.4">
@@ -5330,7 +5334,7 @@
         <v>45</v>
       </c>
       <c r="E268" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.4">
@@ -5347,7 +5351,7 @@
         <v>45</v>
       </c>
       <c r="E269" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.4">
@@ -5364,7 +5368,7 @@
         <v>45</v>
       </c>
       <c r="E270" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.4">
@@ -5381,7 +5385,7 @@
         <v>45</v>
       </c>
       <c r="E271" s="1" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.4">
@@ -5395,10 +5399,10 @@
         <v>3</v>
       </c>
       <c r="D276" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="E276" s="1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="277" spans="1:5" x14ac:dyDescent="0.4">
@@ -5412,10 +5416,10 @@
         <v>5</v>
       </c>
       <c r="D277" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="E277" s="1" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="278" spans="1:5" x14ac:dyDescent="0.4">
@@ -5429,10 +5433,10 @@
         <v>4</v>
       </c>
       <c r="D278" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="E278" s="1" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.4">
@@ -5446,10 +5450,10 @@
         <v>3</v>
       </c>
       <c r="D279" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="E279" s="1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="280" spans="1:5" x14ac:dyDescent="0.4">
@@ -5457,7 +5461,7 @@
         <v>52</v>
       </c>
       <c r="B280" s="1" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C280" s="1">
         <v>5</v>
@@ -5466,7 +5470,7 @@
         <v>55</v>
       </c>
       <c r="E280" s="1" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="281" spans="1:5" x14ac:dyDescent="0.4">
@@ -5483,7 +5487,7 @@
         <v>55</v>
       </c>
       <c r="E281" s="1" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="282" spans="1:5" x14ac:dyDescent="0.4">
@@ -5500,7 +5504,7 @@
         <v>55</v>
       </c>
       <c r="E282" s="1" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.4">
@@ -5517,7 +5521,7 @@
         <v>55</v>
       </c>
       <c r="E285" s="1" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="286" spans="1:5" x14ac:dyDescent="0.4">
@@ -5534,7 +5538,7 @@
         <v>55</v>
       </c>
       <c r="E286" s="1" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="289" spans="1:5" x14ac:dyDescent="0.4">
@@ -5551,7 +5555,7 @@
         <v>64</v>
       </c>
       <c r="E289" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="290" spans="1:5" x14ac:dyDescent="0.4">
@@ -5559,7 +5563,7 @@
         <v>53</v>
       </c>
       <c r="B290" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C290" s="1">
         <v>3</v>
@@ -5568,7 +5572,7 @@
         <v>64</v>
       </c>
       <c r="E290" s="1" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="291" spans="1:5" x14ac:dyDescent="0.4">
@@ -5585,7 +5589,7 @@
         <v>64</v>
       </c>
       <c r="E291" s="1" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="294" spans="1:5" x14ac:dyDescent="0.4">
@@ -5593,7 +5597,7 @@
         <v>54</v>
       </c>
       <c r="B294" s="1" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C294" s="1">
         <v>4</v>
@@ -5602,7 +5606,7 @@
         <v>24</v>
       </c>
       <c r="E294" s="1" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="299" spans="1:5" x14ac:dyDescent="0.4">
@@ -5610,7 +5614,7 @@
         <v>55</v>
       </c>
       <c r="B299" s="1" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C299" s="1">
         <v>4</v>
@@ -5619,7 +5623,7 @@
         <v>30</v>
       </c>
       <c r="E299" s="1" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="301" spans="1:5" x14ac:dyDescent="0.4">
@@ -5627,7 +5631,7 @@
         <v>56</v>
       </c>
       <c r="B301" s="1" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C301" s="1">
         <v>4</v>
@@ -5653,7 +5657,7 @@
         <v>41</v>
       </c>
       <c r="E305" s="1" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="306" spans="1:5" x14ac:dyDescent="0.4">
@@ -5670,7 +5674,7 @@
         <v>41</v>
       </c>
       <c r="E306" s="1" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="308" spans="1:5" x14ac:dyDescent="0.4">
@@ -5678,7 +5682,7 @@
         <v>57</v>
       </c>
       <c r="B308" s="1" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C308" s="1">
         <v>4</v>
@@ -5687,7 +5691,7 @@
         <v>41</v>
       </c>
       <c r="E308" s="1" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="315" spans="1:5" x14ac:dyDescent="0.4">
@@ -5704,7 +5708,7 @@
         <v>49</v>
       </c>
       <c r="E315" s="1" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="316" spans="1:5" x14ac:dyDescent="0.4">
@@ -5718,10 +5722,10 @@
         <v>5</v>
       </c>
       <c r="D316" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="E316" s="1" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="317" spans="1:5" x14ac:dyDescent="0.4">
@@ -5729,16 +5733,16 @@
         <v>60</v>
       </c>
       <c r="B317" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="C317" s="1">
         <v>5</v>
       </c>
       <c r="D317" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="E317" s="1" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="318" spans="1:5" x14ac:dyDescent="0.4">
@@ -5752,10 +5756,10 @@
         <v>4</v>
       </c>
       <c r="D318" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="E318" s="2" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="319" spans="1:5" x14ac:dyDescent="0.4">
@@ -5769,10 +5773,10 @@
         <v>4</v>
       </c>
       <c r="D319" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="E319" s="1" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="320" spans="1:5" x14ac:dyDescent="0.4">
@@ -5786,10 +5790,10 @@
         <v>4</v>
       </c>
       <c r="D320" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="E320" s="1" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="321" spans="1:5" x14ac:dyDescent="0.4">
@@ -5806,7 +5810,7 @@
         <v>55</v>
       </c>
       <c r="E321" s="1" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="322" spans="1:5" x14ac:dyDescent="0.4">
@@ -5814,7 +5818,7 @@
         <v>61</v>
       </c>
       <c r="B322" s="1" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C322" s="1">
         <v>5</v>
@@ -5823,7 +5827,7 @@
         <v>55</v>
       </c>
       <c r="E322" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="323" spans="1:5" x14ac:dyDescent="0.4">
@@ -5840,7 +5844,7 @@
         <v>55</v>
       </c>
       <c r="E323" s="1" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="324" spans="1:5" x14ac:dyDescent="0.4">
@@ -5857,7 +5861,7 @@
         <v>55</v>
       </c>
       <c r="E324" s="1" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="327" spans="1:5" x14ac:dyDescent="0.4">
@@ -5874,7 +5878,7 @@
         <v>64</v>
       </c>
       <c r="E327" s="1" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="328" spans="1:5" x14ac:dyDescent="0.4">
@@ -5891,7 +5895,7 @@
         <v>24</v>
       </c>
       <c r="E328" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="330" spans="1:5" x14ac:dyDescent="0.4">
@@ -5908,7 +5912,7 @@
         <v>24</v>
       </c>
       <c r="E330" s="1" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="331" spans="1:5" x14ac:dyDescent="0.4">
@@ -5916,7 +5920,7 @@
         <v>64</v>
       </c>
       <c r="B331" s="1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="C331" s="1">
         <v>4</v>
@@ -5925,7 +5929,7 @@
         <v>30</v>
       </c>
       <c r="E331" s="1" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="332" spans="1:5" x14ac:dyDescent="0.4">
@@ -5933,7 +5937,7 @@
         <v>64</v>
       </c>
       <c r="B332" s="1" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C332" s="1">
         <v>4</v>
@@ -5942,7 +5946,7 @@
         <v>30</v>
       </c>
       <c r="E332" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="333" spans="1:5" x14ac:dyDescent="0.4">
@@ -5950,7 +5954,7 @@
         <v>64</v>
       </c>
       <c r="B333" s="1" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C333" s="1">
         <v>5</v>
@@ -5959,7 +5963,7 @@
         <v>30</v>
       </c>
       <c r="E333" s="1" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="335" spans="1:5" x14ac:dyDescent="0.4">
@@ -5976,7 +5980,7 @@
         <v>38</v>
       </c>
       <c r="E335" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="337" spans="1:5" x14ac:dyDescent="0.4">
@@ -5993,14 +5997,16 @@
         <v>41</v>
       </c>
       <c r="E337" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="E318" r:id="rId1" xr:uid="{11516621-A74D-46BE-A3CF-DE00ECF7FAD3}"/>
+    <hyperlink ref="E112" r:id="rId2" xr:uid="{4137A055-47B0-4305-AC5F-96059F4CB979}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>